<commit_message>
ADD PREVIEW IMAGE IN DETAILED PHASE, ADD FUNCTION TO DELETE IMAGE, LITTLE TWEAK IN REPORT PAGE
</commit_message>
<xml_diff>
--- a/nhap lieu/nhap lieu tieu chi cua cac bo phan.xlsx
+++ b/nhap lieu/nhap lieu tieu chi cua cac bo phan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="13"/>
+    <workbookView windowWidth="27945" windowHeight="12300" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="xuong1" sheetId="9" r:id="rId1"/>
@@ -10963,10 +10963,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B242"/>
+  <dimension ref="A1:B312"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210:B242"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="B292" sqref="B292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -12909,6 +12909,566 @@
       </c>
       <c r="B242">
         <v>229</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243">
+        <v>71</v>
+      </c>
+      <c r="B243">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244">
+        <v>71</v>
+      </c>
+      <c r="B244">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245">
+        <v>71</v>
+      </c>
+      <c r="B245">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246">
+        <v>71</v>
+      </c>
+      <c r="B246">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247">
+        <v>71</v>
+      </c>
+      <c r="B247">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248">
+        <v>71</v>
+      </c>
+      <c r="B248">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249">
+        <v>71</v>
+      </c>
+      <c r="B249">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250">
+        <v>71</v>
+      </c>
+      <c r="B250">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251">
+        <v>71</v>
+      </c>
+      <c r="B251">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252">
+        <v>71</v>
+      </c>
+      <c r="B252">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253">
+        <v>71</v>
+      </c>
+      <c r="B253">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254">
+        <v>71</v>
+      </c>
+      <c r="B254">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255">
+        <v>71</v>
+      </c>
+      <c r="B255">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256">
+        <v>71</v>
+      </c>
+      <c r="B256">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257">
+        <v>71</v>
+      </c>
+      <c r="B257">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258">
+        <v>71</v>
+      </c>
+      <c r="B258">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259">
+        <v>72</v>
+      </c>
+      <c r="B259">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260">
+        <v>72</v>
+      </c>
+      <c r="B260">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261">
+        <v>72</v>
+      </c>
+      <c r="B261">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262">
+        <v>72</v>
+      </c>
+      <c r="B262">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263">
+        <v>72</v>
+      </c>
+      <c r="B263">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264">
+        <v>72</v>
+      </c>
+      <c r="B264">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265">
+        <v>72</v>
+      </c>
+      <c r="B265">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266">
+        <v>72</v>
+      </c>
+      <c r="B266">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267">
+        <v>72</v>
+      </c>
+      <c r="B267">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268">
+        <v>72</v>
+      </c>
+      <c r="B268">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269">
+        <v>72</v>
+      </c>
+      <c r="B269">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270">
+        <v>72</v>
+      </c>
+      <c r="B270">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271">
+        <v>72</v>
+      </c>
+      <c r="B271">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272">
+        <v>72</v>
+      </c>
+      <c r="B272">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273">
+        <v>72</v>
+      </c>
+      <c r="B273">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274">
+        <v>72</v>
+      </c>
+      <c r="B274">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275">
+        <v>72</v>
+      </c>
+      <c r="B275">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276">
+        <v>72</v>
+      </c>
+      <c r="B276">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277">
+        <v>72</v>
+      </c>
+      <c r="B277">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278">
+        <v>72</v>
+      </c>
+      <c r="B278">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279">
+        <v>72</v>
+      </c>
+      <c r="B279">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280">
+        <v>72</v>
+      </c>
+      <c r="B280">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281">
+        <v>72</v>
+      </c>
+      <c r="B281">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282">
+        <v>72</v>
+      </c>
+      <c r="B282">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283">
+        <v>72</v>
+      </c>
+      <c r="B283">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284">
+        <v>72</v>
+      </c>
+      <c r="B284">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285">
+        <v>72</v>
+      </c>
+      <c r="B285">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286">
+        <v>72</v>
+      </c>
+      <c r="B286">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287">
+        <v>72</v>
+      </c>
+      <c r="B287">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288">
+        <v>72</v>
+      </c>
+      <c r="B288">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289">
+        <v>72</v>
+      </c>
+      <c r="B289">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290">
+        <v>72</v>
+      </c>
+      <c r="B290">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291">
+        <v>72</v>
+      </c>
+      <c r="B291">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292">
+        <v>72</v>
+      </c>
+      <c r="B292">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2">
+      <c r="A293">
+        <v>73</v>
+      </c>
+      <c r="B293">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294">
+        <v>73</v>
+      </c>
+      <c r="B294">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295">
+        <v>73</v>
+      </c>
+      <c r="B295">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296">
+        <v>73</v>
+      </c>
+      <c r="B296">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297">
+        <v>73</v>
+      </c>
+      <c r="B297">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298">
+        <v>73</v>
+      </c>
+      <c r="B298">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299">
+        <v>73</v>
+      </c>
+      <c r="B299">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300">
+        <v>73</v>
+      </c>
+      <c r="B300">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2">
+      <c r="A301">
+        <v>73</v>
+      </c>
+      <c r="B301">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2">
+      <c r="A302">
+        <v>73</v>
+      </c>
+      <c r="B302">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2">
+      <c r="A303">
+        <v>73</v>
+      </c>
+      <c r="B303">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2">
+      <c r="A304">
+        <v>73</v>
+      </c>
+      <c r="B304">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2">
+      <c r="A305">
+        <v>73</v>
+      </c>
+      <c r="B305">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2">
+      <c r="A306">
+        <v>73</v>
+      </c>
+      <c r="B306">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2">
+      <c r="A307">
+        <v>73</v>
+      </c>
+      <c r="B307">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2">
+      <c r="A308">
+        <v>73</v>
+      </c>
+      <c r="B308">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2">
+      <c r="A309">
+        <v>73</v>
+      </c>
+      <c r="B309">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2">
+      <c r="A310">
+        <v>73</v>
+      </c>
+      <c r="B310">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2">
+      <c r="A311">
+        <v>73</v>
+      </c>
+      <c r="B311">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2">
+      <c r="A312">
+        <v>73</v>
+      </c>
+      <c r="B312">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>